<commit_message>
Added Sx relations from Wang thesis
</commit_message>
<xml_diff>
--- a/inputsGit/SI_percent_by_edagrid.xlsx
+++ b/inputsGit/SI_percent_by_edagrid.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\SIBEC_Modelled\working\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\SIBEC_Modelled\inputsGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D198424-2BD3-4DE5-8C83-A70A34DA01AD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF3E710-69C7-4056-AA0D-9FBD3AB0BFE2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="1755" windowWidth="16485" windowHeight="15870" activeTab="10" xr2:uid="{C44777EE-7EF2-477D-9B72-BFFF0EC7632C}"/>
+    <workbookView xWindow="45435" yWindow="2850" windowWidth="21855" windowHeight="15870" activeTab="11" xr2:uid="{C44777EE-7EF2-477D-9B72-BFFF0EC7632C}"/>
   </bookViews>
   <sheets>
     <sheet name="Ba" sheetId="10" r:id="rId1"/>
@@ -325,6 +325,87 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94D73C13-5660-4971-A7EA-344CD9C263DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4410075" y="371475"/>
+          <a:ext cx="2743200" cy="1200150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>From GG Wang 1993 thesis.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>table 4.21</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1029,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07132632-98F5-41C9-B7B8-AE6846773071}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1269,87 +1350,238 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE4AA88-8C45-4179-B9D3-DBCCEFC23EB4}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="9.140625" style="2"/>
+    <col min="1" max="6" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="B5" s="4">
+        <v>0.67</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.67</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="B6" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="B7" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="B8" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="B9" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.92</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.92</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="B10" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="D10" s="4">
+        <v>60</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.77</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.77</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Trying to fix tables
</commit_message>
<xml_diff>
--- a/inputsGit/SI_percent_by_edagrid.xlsx
+++ b/inputsGit/SI_percent_by_edagrid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\SIBEC_Modelled\working\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirid\Desktop\SIBEC_Modelled\inputsGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D198424-2BD3-4DE5-8C83-A70A34DA01AD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5D94CE-17A1-49A8-BBAC-51AEB7EF7FF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="1755" windowWidth="16485" windowHeight="15870" activeTab="10" xr2:uid="{C44777EE-7EF2-477D-9B72-BFFF0EC7632C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{C44777EE-7EF2-477D-9B72-BFFF0EC7632C}"/>
   </bookViews>
   <sheets>
     <sheet name="Ba" sheetId="10" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <sheet name="Ra" sheetId="19" r:id="rId19"/>
     <sheet name="Bp" sheetId="20" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -325,6 +325,87 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94D73C13-5660-4971-A7EA-344CD9C263DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4410075" y="371475"/>
+          <a:ext cx="2743200" cy="1200150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>From GG Wang 1993 thesis.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>table 4.21</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -707,12 +788,12 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="9.140625" style="4"/>
+    <col min="2" max="6" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -732,7 +813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -752,7 +833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -772,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -792,7 +873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -812,7 +893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -832,7 +913,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -852,7 +933,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -872,7 +953,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -892,7 +973,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -912,7 +993,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -945,12 +1026,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="9.140625" style="2"/>
+    <col min="2" max="6" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -970,52 +1051,52 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1029,18 +1110,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07132632-98F5-41C9-B7B8-AE6846773071}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" customWidth="1"/>
-    <col min="2" max="6" width="8.5703125" customWidth="1"/>
-    <col min="16" max="16" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="6" width="8.5546875" customWidth="1"/>
+    <col min="16" max="16" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1060,7 +1141,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1080,7 +1161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1100,7 +1181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1120,7 +1201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1140,7 +1221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1160,7 +1241,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1180,7 +1261,7 @@
         <v>0.82926829268292679</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1200,7 +1281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1220,7 +1301,7 @@
         <v>0.97560975609756095</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1240,7 +1321,7 @@
         <v>0.6097560975609756</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1270,86 +1351,237 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="9.140625" style="2"/>
+    <col min="1" max="6" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B5" s="4">
+        <v>0.67</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.67</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B6" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B7" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B8" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B9" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.92</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B10" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="D10" s="4">
+        <v>60</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.77</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1361,12 +1593,12 @@
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="9.140625" style="4"/>
+    <col min="2" max="6" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1386,7 +1618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1406,7 +1638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1426,7 +1658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1446,7 +1678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1466,7 +1698,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1486,7 +1718,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1506,7 +1738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1526,7 +1758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1546,7 +1778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1566,7 +1798,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1600,12 +1832,12 @@
       <selection activeCell="B1" sqref="B1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="9.140625" style="4"/>
+    <col min="2" max="6" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1625,7 +1857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1645,7 +1877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1665,7 +1897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1685,7 +1917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1705,7 +1937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1725,7 +1957,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1745,7 +1977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1765,7 +1997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1785,7 +2017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1805,7 +2037,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1838,12 +2070,12 @@
       <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="9.140625" style="4"/>
+    <col min="2" max="6" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1863,7 +2095,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1883,7 +2115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1903,7 +2135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1923,7 +2155,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1943,7 +2175,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1963,7 +2195,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1983,7 +2215,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2003,7 +2235,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2023,7 +2255,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2043,7 +2275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2076,12 +2308,12 @@
       <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="9.140625" style="4"/>
+    <col min="2" max="6" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2101,7 +2333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2121,7 +2353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2141,7 +2373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2161,7 +2393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2181,7 +2413,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2201,7 +2433,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2221,7 +2453,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2241,7 +2473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2261,7 +2493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2281,7 +2513,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2314,12 +2546,12 @@
       <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="9.140625" style="4"/>
+    <col min="2" max="6" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2339,7 +2571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2359,7 +2591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2379,7 +2611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2399,7 +2631,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2419,7 +2651,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2439,7 +2671,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2459,7 +2691,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2479,7 +2711,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2499,7 +2731,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2519,7 +2751,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2552,12 +2784,12 @@
       <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="9.140625" style="4"/>
+    <col min="2" max="6" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2577,7 +2809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2597,7 +2829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2617,7 +2849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2637,7 +2869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2657,7 +2889,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2677,7 +2909,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2697,7 +2929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2717,7 +2949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2737,7 +2969,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2757,7 +2989,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2790,12 +3022,12 @@
       <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="9.140625" style="4"/>
+    <col min="2" max="6" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2815,7 +3047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2835,7 +3067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2855,7 +3087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2875,7 +3107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2895,7 +3127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2915,7 +3147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2935,7 +3167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2955,7 +3187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2975,7 +3207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2995,7 +3227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -3028,12 +3260,12 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="9.140625" style="2"/>
+    <col min="2" max="6" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -3053,7 +3285,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3073,7 +3305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3093,7 +3325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3113,7 +3345,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3133,7 +3365,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3153,7 +3385,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3173,7 +3405,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3193,7 +3425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -3213,7 +3445,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3233,7 +3465,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -3267,9 +3499,9 @@
       <selection sqref="A1:F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -3289,7 +3521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3309,7 +3541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3329,7 +3561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3349,7 +3581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3369,7 +3601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3389,7 +3621,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3409,7 +3641,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3429,7 +3661,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -3449,7 +3681,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3469,7 +3701,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -3502,12 +3734,12 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="9.140625" style="2"/>
+    <col min="2" max="6" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -3527,52 +3759,52 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -3590,9 +3822,9 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -3612,7 +3844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3632,7 +3864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3652,7 +3884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3672,7 +3904,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3692,7 +3924,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3712,7 +3944,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3732,7 +3964,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3753,7 +3985,7 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -3773,7 +4005,7 @@
         <v>0.99378881987577627</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3793,7 +4025,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -3813,7 +4045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L20" s="1"/>
     </row>
   </sheetData>
@@ -3825,16 +4057,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0711EA2F-0A01-497C-9996-C755ECE08F8E}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="9.140625" style="2"/>
+    <col min="2" max="6" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -3854,7 +4086,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3874,7 +4106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3894,7 +4126,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3914,7 +4146,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3934,7 +4166,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3954,7 +4186,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3962,7 +4194,7 @@
         <v>0.4</v>
       </c>
       <c r="C7" s="3">
-        <v>7</v>
+        <v>0.7</v>
       </c>
       <c r="D7" s="3">
         <v>0.9</v>
@@ -3974,7 +4206,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3994,7 +4226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -4014,7 +4246,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -4034,7 +4266,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -4067,12 +4299,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="9.140625" style="2"/>
+    <col min="2" max="6" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -4092,52 +4324,52 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -4155,13 +4387,13 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="10.85546875" style="4" customWidth="1"/>
-    <col min="16" max="16" width="49.28515625" customWidth="1"/>
+    <col min="2" max="6" width="10.88671875" style="4" customWidth="1"/>
+    <col min="16" max="16" width="49.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4178,7 +4410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4198,7 +4430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4218,7 +4450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4238,7 +4470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -4258,7 +4490,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -4278,7 +4510,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -4298,7 +4530,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4318,7 +4550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -4338,7 +4570,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -4358,7 +4590,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -4392,12 +4624,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="9.140625" style="2"/>
+    <col min="2" max="6" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -4417,52 +4649,52 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -4480,12 +4712,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="9.140625" style="2"/>
+    <col min="2" max="6" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -4505,52 +4737,52 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
added values for Bl and Pl. Approximations only
</commit_message>
<xml_diff>
--- a/inputsGit/SI_percent_by_edagrid.xlsx
+++ b/inputsGit/SI_percent_by_edagrid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirid\Desktop\SIBEC_Modelled\inputsGit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\SIBEC_Modelled\inputsGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE49F17-262B-4AD9-8D3D-F63C150099A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8463A9B2-A897-49AE-97F6-3AC1DBCD0D19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="11" xr2:uid="{C44777EE-7EF2-477D-9B72-BFFF0EC7632C}"/>
+    <workbookView xWindow="11580" yWindow="2655" windowWidth="21855" windowHeight="15870" firstSheet="1" activeTab="2" xr2:uid="{C44777EE-7EF2-477D-9B72-BFFF0EC7632C}"/>
   </bookViews>
   <sheets>
     <sheet name="Ba" sheetId="10" r:id="rId1"/>
@@ -785,15 +785,15 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="C7" sqref="C7:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="9.109375" style="4"/>
+    <col min="2" max="6" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -813,7 +813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -833,7 +833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -853,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -873,7 +873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -893,87 +893,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="C6" s="4">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="D6" s="4">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="E6" s="4">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="F6" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="4">
-        <v>70</v>
+        <v>0.7</v>
       </c>
       <c r="C7" s="4">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="D7" s="4">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E7" s="4">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F7" s="4">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="4">
-        <v>70</v>
+        <v>0.7</v>
       </c>
       <c r="C8" s="4">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="D8" s="4">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E8" s="4">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F8" s="4">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="4">
-        <v>70</v>
+        <v>0.7</v>
       </c>
       <c r="C9" s="4">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="D9" s="4">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E9" s="4">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F9" s="4">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -984,16 +984,16 @@
         <v>0</v>
       </c>
       <c r="D10" s="4">
-        <v>70</v>
+        <v>0.7</v>
       </c>
       <c r="E10" s="4">
-        <v>70</v>
+        <v>0.7</v>
       </c>
       <c r="F10" s="4">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1026,12 +1026,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="9.109375" style="2"/>
+    <col min="2" max="6" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1051,52 +1051,52 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1114,14 +1114,14 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="6" width="8.5546875" customWidth="1"/>
-    <col min="16" max="16" width="30.33203125" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="6" width="8.5703125" customWidth="1"/>
+    <col min="16" max="16" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>0.82926829268292679</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>0.97560975609756095</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>0.6097560975609756</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1350,14 +1350,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE4AA88-8C45-4179-B9D3-DBCCEFC23EB4}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="9.109375" style="4"/>
+    <col min="1" max="6" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -1591,12 +1591,12 @@
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="9.109375" style="4"/>
+    <col min="2" max="6" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1830,12 +1830,12 @@
       <selection activeCell="B1" sqref="B1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="9.109375" style="4"/>
+    <col min="2" max="6" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2068,12 +2068,12 @@
       <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="9.109375" style="4"/>
+    <col min="2" max="6" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2306,12 +2306,12 @@
       <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="9.109375" style="4"/>
+    <col min="2" max="6" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2544,12 +2544,12 @@
       <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="9.109375" style="4"/>
+    <col min="2" max="6" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2782,12 +2782,12 @@
       <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="9.109375" style="4"/>
+    <col min="2" max="6" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -3020,12 +3020,12 @@
       <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="9.109375" style="4"/>
+    <col min="2" max="6" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -3258,12 +3258,12 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="9.109375" style="2"/>
+    <col min="2" max="6" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -3497,9 +3497,9 @@
       <selection sqref="A1:F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -3728,16 +3728,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C93E88E-3361-4DD3-A238-C02D797C2095}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="9.109375" style="2"/>
+    <col min="2" max="6" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -3757,54 +3757,204 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3820,9 +3970,9 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -3842,7 +3992,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3862,7 +4012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3882,7 +4032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3902,7 +4052,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3922,7 +4072,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3942,7 +4092,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3962,7 +4112,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3983,7 +4133,7 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -4003,7 +4153,7 @@
         <v>0.99378881987577627</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -4023,7 +4173,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -4043,7 +4193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L20" s="1"/>
     </row>
   </sheetData>
@@ -4059,12 +4209,12 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="9.109375" style="2"/>
+    <col min="2" max="6" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -4084,7 +4234,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4104,7 +4254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4124,7 +4274,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4144,7 +4294,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -4164,7 +4314,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -4184,7 +4334,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -4204,7 +4354,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4224,7 +4374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -4244,7 +4394,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -4264,7 +4414,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -4297,12 +4447,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="9.109375" style="2"/>
+    <col min="2" max="6" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -4322,52 +4472,52 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -4385,13 +4535,13 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="10.88671875" style="4" customWidth="1"/>
-    <col min="16" max="16" width="49.33203125" customWidth="1"/>
+    <col min="2" max="6" width="10.85546875" style="4" customWidth="1"/>
+    <col min="16" max="16" width="49.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4408,7 +4558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4428,7 +4578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4448,7 +4598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4468,7 +4618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -4488,7 +4638,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -4508,7 +4658,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -4528,7 +4678,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4548,7 +4698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -4568,7 +4718,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -4588,7 +4738,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -4622,12 +4772,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="9.109375" style="2"/>
+    <col min="2" max="6" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -4647,52 +4797,52 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -4707,15 +4857,15 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="9.109375" style="2"/>
+    <col min="2" max="6" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -4735,54 +4885,204 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added values for Pl ande Lw
</commit_message>
<xml_diff>
--- a/inputsGit/SI_percent_by_edagrid.xlsx
+++ b/inputsGit/SI_percent_by_edagrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\SIBEC_Modelled\inputsGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8463A9B2-A897-49AE-97F6-3AC1DBCD0D19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF01C5D-9CAF-404A-8E49-8D75A3D62AE5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="2655" windowWidth="21855" windowHeight="15870" firstSheet="1" activeTab="2" xr2:uid="{C44777EE-7EF2-477D-9B72-BFFF0EC7632C}"/>
+    <workbookView xWindow="41985" yWindow="2835" windowWidth="21855" windowHeight="15870" firstSheet="1" activeTab="15" xr2:uid="{C44777EE-7EF2-477D-9B72-BFFF0EC7632C}"/>
   </bookViews>
   <sheets>
     <sheet name="Ba" sheetId="10" r:id="rId1"/>
@@ -249,86 +249,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD4D7B04-487B-4E79-8467-5602030DA04C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4838700" y="190500"/>
-          <a:ext cx="2847975" cy="990600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>from Kayahara and SIBEC</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t> CWHvm1</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-CA" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -405,7 +325,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2302,7 +2222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7531EF36-4035-4AFE-9241-025B586BB1A0}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
@@ -3728,7 +3648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C93E88E-3361-4DD3-A238-C02D797C2095}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -4532,11 +4452,12 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="6" width="10.85546875" style="4" customWidth="1"/>
     <col min="16" max="16" width="49.28515625" customWidth="1"/>
   </cols>
@@ -4559,7 +4480,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4">
@@ -4579,7 +4500,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4">
@@ -4599,7 +4520,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="4">
@@ -4619,7 +4540,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="4">
@@ -4639,7 +4560,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4">
@@ -4659,7 +4580,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="4">
@@ -4679,7 +4600,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="4">
@@ -4699,7 +4620,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="4">
@@ -4719,7 +4640,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="4">
@@ -4739,7 +4660,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="4">
@@ -4760,7 +4681,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4769,7 +4689,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4801,50 +4721,200 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
+      <c r="B5" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
+      <c r="B6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
+      <c r="B7" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
+      <c r="B8" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the Bl % to better match data
</commit_message>
<xml_diff>
--- a/inputsGit/SI_percent_by_edagrid.xlsx
+++ b/inputsGit/SI_percent_by_edagrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\SIBEC_Modelled\inputsGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF01C5D-9CAF-404A-8E49-8D75A3D62AE5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714A2FE4-5F16-4DE0-BB18-E9ABF01E1806}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41985" yWindow="2835" windowWidth="21855" windowHeight="15870" firstSheet="1" activeTab="15" xr2:uid="{C44777EE-7EF2-477D-9B72-BFFF0EC7632C}"/>
+    <workbookView xWindow="19320" yWindow="4125" windowWidth="21855" windowHeight="15870" firstSheet="1" activeTab="2" xr2:uid="{C44777EE-7EF2-477D-9B72-BFFF0EC7632C}"/>
   </bookViews>
   <sheets>
     <sheet name="Ba" sheetId="10" r:id="rId1"/>
@@ -2222,7 +2222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7531EF36-4035-4AFE-9241-025B586BB1A0}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
@@ -3648,8 +3648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C93E88E-3361-4DD3-A238-C02D797C2095}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3765,16 +3765,16 @@
         <v>0.6</v>
       </c>
       <c r="C6" s="4">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="D6" s="4">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="E6" s="4">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="F6" s="4">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3788,7 +3788,7 @@
         <v>0.8</v>
       </c>
       <c r="D7" s="4">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="E7" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
update of LW edatope
</commit_message>
<xml_diff>
--- a/inputsGit/SI_percent_by_edagrid.xlsx
+++ b/inputsGit/SI_percent_by_edagrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\SIBEC_Modelled\inputsGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714A2FE4-5F16-4DE0-BB18-E9ABF01E1806}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5210DB54-C982-4EA1-AC23-9DA68092BAA9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19320" yWindow="4125" windowWidth="21855" windowHeight="15870" firstSheet="1" activeTab="2" xr2:uid="{C44777EE-7EF2-477D-9B72-BFFF0EC7632C}"/>
+    <workbookView xWindow="44145" yWindow="3465" windowWidth="21855" windowHeight="15870" firstSheet="1" activeTab="7" xr2:uid="{C44777EE-7EF2-477D-9B72-BFFF0EC7632C}"/>
   </bookViews>
   <sheets>
     <sheet name="Ba" sheetId="10" r:id="rId1"/>
@@ -249,6 +249,86 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5CBD06A-21A7-4B22-8D3D-9D5CE0BEB8CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4857750" y="381000"/>
+          <a:ext cx="3905250" cy="1247775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>Table 5.3</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t> in New's thesis</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -325,7 +405,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3175,7 +3255,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3648,8 +3728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C93E88E-3361-4DD3-A238-C02D797C2095}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4688,8 +4768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{559F736D-8FD6-46ED-9A45-F3CB0139281B}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4742,19 +4822,19 @@
         <v>6</v>
       </c>
       <c r="B3" s="4">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="C3" s="4">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="D3" s="4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E3" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F3" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4762,19 +4842,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C4" s="4">
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D4" s="4">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E4" s="4">
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="F4" s="4">
-        <v>0</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -4782,19 +4862,19 @@
         <v>8</v>
       </c>
       <c r="B5" s="4">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="C5" s="4">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
       <c r="D5" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="E5" s="4">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="F5" s="4">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -4802,10 +4882,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="4">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="C6" s="4">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="D6" s="4">
         <v>0.85</v>
@@ -4822,19 +4902,19 @@
         <v>10</v>
       </c>
       <c r="B7" s="4">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="C7" s="4">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="D7" s="4">
         <v>0.9</v>
       </c>
       <c r="E7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="F7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -4842,19 +4922,19 @@
         <v>14</v>
       </c>
       <c r="B8" s="4">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
       <c r="C8" s="4">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="D8" s="4">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="E8" s="4">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="F8" s="4">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -4862,19 +4942,19 @@
         <v>11</v>
       </c>
       <c r="B9" s="4">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="C9" s="4">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="D9" s="4">
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="E9" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="F9" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -4882,19 +4962,19 @@
         <v>12</v>
       </c>
       <c r="B10" s="4">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="C10" s="4">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="D10" s="4">
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="E10" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="F10" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -4919,6 +4999,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Working table of percent maxSI by edatopic cell
</commit_message>
<xml_diff>
--- a/inputsGit/SI_percent_by_edagrid.xlsx
+++ b/inputsGit/SI_percent_by_edagrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\SIBEC_Modelled\inputsGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5210DB54-C982-4EA1-AC23-9DA68092BAA9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC259FE-0793-4AEB-A2C8-260DB9FC4EF5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44145" yWindow="3465" windowWidth="21855" windowHeight="15870" firstSheet="1" activeTab="7" xr2:uid="{C44777EE-7EF2-477D-9B72-BFFF0EC7632C}"/>
+    <workbookView xWindow="8250" yWindow="1890" windowWidth="21855" windowHeight="17760" firstSheet="1" activeTab="9" xr2:uid="{C44777EE-7EF2-477D-9B72-BFFF0EC7632C}"/>
   </bookViews>
   <sheets>
     <sheet name="Ba" sheetId="10" r:id="rId1"/>
@@ -22,17 +22,18 @@
     <sheet name="Hw" sheetId="1" r:id="rId7"/>
     <sheet name="Lw" sheetId="17" r:id="rId8"/>
     <sheet name="Pl" sheetId="5" r:id="rId9"/>
-    <sheet name="Py" sheetId="7" r:id="rId10"/>
-    <sheet name="Ss" sheetId="2" r:id="rId11"/>
-    <sheet name="Sx" sheetId="6" r:id="rId12"/>
-    <sheet name="Yc" sheetId="15" r:id="rId13"/>
-    <sheet name="Ac" sheetId="14" r:id="rId14"/>
-    <sheet name="At" sheetId="18" r:id="rId15"/>
-    <sheet name="Dr" sheetId="12" r:id="rId16"/>
-    <sheet name="Ep" sheetId="13" r:id="rId17"/>
-    <sheet name="Mb" sheetId="16" r:id="rId18"/>
-    <sheet name="Ra" sheetId="19" r:id="rId19"/>
-    <sheet name="Bp" sheetId="20" r:id="rId20"/>
+    <sheet name="Pw" sheetId="21" r:id="rId10"/>
+    <sheet name="Py" sheetId="7" r:id="rId11"/>
+    <sheet name="Ss" sheetId="2" r:id="rId12"/>
+    <sheet name="Sx" sheetId="6" r:id="rId13"/>
+    <sheet name="Yc" sheetId="15" r:id="rId14"/>
+    <sheet name="Ac" sheetId="14" r:id="rId15"/>
+    <sheet name="At" sheetId="18" r:id="rId16"/>
+    <sheet name="Dr" sheetId="12" r:id="rId17"/>
+    <sheet name="Ep" sheetId="13" r:id="rId18"/>
+    <sheet name="Mb" sheetId="16" r:id="rId19"/>
+    <sheet name="Ra" sheetId="19" r:id="rId20"/>
+    <sheet name="Bp" sheetId="20" r:id="rId21"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="16">
   <si>
     <t>A</t>
   </si>
@@ -1019,11 +1020,246 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4953CF86-436B-4117-96BF-9FCE03BF4B07}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0375AB61-F097-4CA1-BB9B-4DA4E8FB6CA1}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,50 +1291,200 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1106,7 +1492,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07132632-98F5-41C9-B7B8-AE6846773071}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -1346,7 +1732,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE4AA88-8C45-4179-B9D3-DBCCEFC23EB4}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -1583,7 +1969,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95792EA-508C-4FAB-9880-E7E4A88B6EB9}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -1822,7 +2208,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3BD4163-0421-4FFD-95C4-3CE5C3514F0C}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -2060,12 +2446,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0663FF-CDCA-49DE-9890-01552EBC4BB4}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection sqref="A1:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2144,13 +2530,13 @@
         <v>0.3</v>
       </c>
       <c r="D4" s="4">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="E4" s="4">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="F4" s="4">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2161,13 +2547,13 @@
         <v>0.3</v>
       </c>
       <c r="C5" s="4">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="D5" s="4">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="E5" s="4">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="F5" s="4">
         <v>0.7</v>
@@ -2178,19 +2564,19 @@
         <v>9</v>
       </c>
       <c r="B6" s="4">
-        <v>0.3</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C6" s="4">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="D6" s="4">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E6" s="4">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="F6" s="4">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2198,19 +2584,19 @@
         <v>10</v>
       </c>
       <c r="B7" s="4">
-        <v>0.3</v>
+        <v>0.65</v>
       </c>
       <c r="C7" s="4">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="D7" s="4">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="E7" s="4">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="F7" s="4">
-        <v>0.7</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2218,19 +2604,19 @@
         <v>14</v>
       </c>
       <c r="B8" s="4">
-        <v>0.3</v>
+        <v>0.65</v>
       </c>
       <c r="C8" s="4">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
       <c r="D8" s="4">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="E8" s="4">
-        <v>0.7</v>
+        <v>0.95</v>
       </c>
       <c r="F8" s="4">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2298,7 +2684,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7531EF36-4035-4AFE-9241-025B586BB1A0}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -2536,12 +2922,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D1A95C2-1624-41ED-ACAD-A32382F3B6BB}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2614,19 +3000,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C4" s="4">
         <v>0.3</v>
       </c>
       <c r="D4" s="4">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="E4" s="4">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="F4" s="4">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2634,16 +3020,16 @@
         <v>8</v>
       </c>
       <c r="B5" s="4">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C5" s="4">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="D5" s="4">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="E5" s="4">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="F5" s="4">
         <v>0.7</v>
@@ -2654,19 +3040,19 @@
         <v>9</v>
       </c>
       <c r="B6" s="4">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="C6" s="4">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="D6" s="4">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="E6" s="4">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="F6" s="4">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2674,19 +3060,19 @@
         <v>10</v>
       </c>
       <c r="B7" s="4">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C7" s="4">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="D7" s="4">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="E7" s="4">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="F7" s="4">
-        <v>0.7</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2694,19 +3080,19 @@
         <v>14</v>
       </c>
       <c r="B8" s="4">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C8" s="4">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
       <c r="D8" s="4">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E8" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="F8" s="4">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2714,13 +3100,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="4">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="C9" s="4">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="D9" s="4">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="E9" s="4">
         <v>0.7</v>
@@ -2737,16 +3123,16 @@
         <v>0</v>
       </c>
       <c r="C10" s="4">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="D10" s="4">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="E10" s="4">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="F10" s="4">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2774,7 +3160,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3172A72E-40EB-4724-8228-59CA56AA7FC6}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -2985,244 +3371,6 @@
       </c>
       <c r="F10" s="4">
         <v>0.3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5277536-7F28-432C-B85E-FF4CDCE31DFD}">
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="6" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="4">
-        <v>0</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="4">
-        <v>0</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3490,6 +3638,244 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5277536-7F28-432C-B85E-FF4CDCE31DFD}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="6" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8BCF85A-F29E-4B12-A803-7B01DEE1E39A}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -4206,7 +4592,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection sqref="A1:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4768,7 +5154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{559F736D-8FD6-46ED-9A45-F3CB0139281B}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added in some additional missed species
</commit_message>
<xml_diff>
--- a/inputsGit/SI_percent_by_edagrid.xlsx
+++ b/inputsGit/SI_percent_by_edagrid.xlsx
@@ -1,39 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\SIBEC_Modelled\inputsGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC259FE-0793-4AEB-A2C8-260DB9FC4EF5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DE4417-1044-4526-8C29-C486DAE1DDE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8250" yWindow="1890" windowWidth="21855" windowHeight="17760" firstSheet="1" activeTab="9" xr2:uid="{C44777EE-7EF2-477D-9B72-BFFF0EC7632C}"/>
+    <workbookView xWindow="56760" yWindow="1005" windowWidth="17685" windowHeight="18930" firstSheet="5" activeTab="13" xr2:uid="{C44777EE-7EF2-477D-9B72-BFFF0EC7632C}"/>
   </bookViews>
   <sheets>
     <sheet name="Ba" sheetId="10" r:id="rId1"/>
     <sheet name="Bg" sheetId="11" r:id="rId2"/>
     <sheet name="Bl" sheetId="9" r:id="rId3"/>
     <sheet name="Cw" sheetId="3" r:id="rId4"/>
-    <sheet name="Fd" sheetId="4" r:id="rId5"/>
+    <sheet name="Fd" sheetId="22" r:id="rId5"/>
     <sheet name="Hm" sheetId="8" r:id="rId6"/>
     <sheet name="Hw" sheetId="1" r:id="rId7"/>
-    <sheet name="Lw" sheetId="17" r:id="rId8"/>
-    <sheet name="Pl" sheetId="5" r:id="rId9"/>
-    <sheet name="Pw" sheetId="21" r:id="rId10"/>
-    <sheet name="Py" sheetId="7" r:id="rId11"/>
-    <sheet name="Ss" sheetId="2" r:id="rId12"/>
-    <sheet name="Sx" sheetId="6" r:id="rId13"/>
-    <sheet name="Yc" sheetId="15" r:id="rId14"/>
-    <sheet name="Ac" sheetId="14" r:id="rId15"/>
-    <sheet name="At" sheetId="18" r:id="rId16"/>
-    <sheet name="Dr" sheetId="12" r:id="rId17"/>
-    <sheet name="Ep" sheetId="13" r:id="rId18"/>
-    <sheet name="Mb" sheetId="16" r:id="rId19"/>
-    <sheet name="Ra" sheetId="19" r:id="rId20"/>
-    <sheet name="Bp" sheetId="20" r:id="rId21"/>
+    <sheet name="La" sheetId="24" r:id="rId8"/>
+    <sheet name="Lw" sheetId="17" r:id="rId9"/>
+    <sheet name="Pa" sheetId="23" r:id="rId10"/>
+    <sheet name="Pl" sheetId="5" r:id="rId11"/>
+    <sheet name="Pw" sheetId="21" r:id="rId12"/>
+    <sheet name="Py" sheetId="7" r:id="rId13"/>
+    <sheet name="Sb" sheetId="25" r:id="rId14"/>
+    <sheet name="Ss" sheetId="2" r:id="rId15"/>
+    <sheet name="Sx" sheetId="6" r:id="rId16"/>
+    <sheet name="Yc" sheetId="15" r:id="rId17"/>
+    <sheet name="Ac" sheetId="14" r:id="rId18"/>
+    <sheet name="At" sheetId="18" r:id="rId19"/>
+    <sheet name="Dr" sheetId="12" r:id="rId20"/>
+    <sheet name="Ep" sheetId="13" r:id="rId21"/>
+    <sheet name="Mb" sheetId="16" r:id="rId22"/>
+    <sheet name="Ra" sheetId="19" r:id="rId23"/>
+    <sheet name="Bp" sheetId="20" r:id="rId24"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -51,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="16">
   <si>
     <t>A</t>
   </si>
@@ -1020,246 +1023,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4953CF86-436B-4117-96BF-9FCE03BF4B07}">
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.7</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.85</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.7</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="3">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="3">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0375AB61-F097-4CA1-BB9B-4DA4E8FB6CA1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25F4FD76-F19D-40EF-915A-A0F6EB6E36A8}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,16 +1083,16 @@
         <v>0</v>
       </c>
       <c r="C3" s="4">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="D3" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E3" s="4">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="F3" s="4">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1332,19 +1100,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="C4" s="4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D4" s="4">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="E4" s="4">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="F4" s="4">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1352,19 +1120,19 @@
         <v>8</v>
       </c>
       <c r="B5" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C5" s="4">
         <v>0.6</v>
       </c>
       <c r="D5" s="4">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="E5" s="4">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="F5" s="4">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1372,13 +1140,13 @@
         <v>9</v>
       </c>
       <c r="B6" s="4">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="C6" s="4">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="D6" s="4">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="E6" s="4">
         <v>1</v>
@@ -1392,19 +1160,19 @@
         <v>10</v>
       </c>
       <c r="B7" s="4">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="C7" s="4">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="D7" s="4">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E7" s="4">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="F7" s="4">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1412,19 +1180,19 @@
         <v>14</v>
       </c>
       <c r="B8" s="4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="C8" s="4">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="D8" s="4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E8" s="4">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="F8" s="4">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1465,6 +1233,244 @@
       </c>
       <c r="F10" s="4">
         <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6250CC1C-01D0-42DD-AC51-C4DB5F2138AA}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="6" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1493,6 +1499,717 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4953CF86-436B-4117-96BF-9FCE03BF4B07}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0375AB61-F097-4CA1-BB9B-4DA4E8FB6CA1}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="6" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A0336A-0F83-42F2-B3CC-E642C18C6FC6}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07132632-98F5-41C9-B7B8-AE6846773071}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -1732,7 +2449,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE4AA88-8C45-4179-B9D3-DBCCEFC23EB4}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -1969,7 +2686,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95792EA-508C-4FAB-9880-E7E4A88B6EB9}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -2208,7 +2925,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3BD4163-0421-4FFD-95C4-3CE5C3514F0C}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -2446,7 +3163,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0663FF-CDCA-49DE-9890-01552EBC4BB4}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -2657,720 +3374,6 @@
       </c>
       <c r="F10" s="4">
         <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7531EF36-4035-4AFE-9241-025B586BB1A0}">
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="6" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.85</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D1A95C2-1624-41ED-ACAD-A32382F3B6BB}">
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="6" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0.35</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.65</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0.45</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.85</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="4">
-        <v>0.45</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0.85</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="4">
-        <v>0</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3172A72E-40EB-4724-8228-59CA56AA7FC6}">
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="6" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="E7" s="4">
-        <v>1</v>
-      </c>
-      <c r="F7" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="4">
-        <v>0</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="4">
-        <v>0</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0.3</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3638,6 +3641,720 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7531EF36-4035-4AFE-9241-025B586BB1A0}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="6" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D1A95C2-1624-41ED-ACAD-A32382F3B6BB}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="6" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.35</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3172A72E-40EB-4724-8228-59CA56AA7FC6}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="6" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5277536-7F28-432C-B85E-FF4CDCE31DFD}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -3875,7 +4592,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8BCF85A-F29E-4B12-A803-7B01DEE1E39A}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -4588,11 +5305,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0711EA2F-0A01-497C-9996-C755ECE08F8E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A36274-EA7F-44AE-83E3-428B3701CBE4}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F11"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4830,7 +5547,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4862,50 +5579,200 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
+      <c r="B5" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
+      <c r="B6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
+      <c r="B7" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
+      <c r="B8" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
+      <c r="B9" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>6.811989100817438E-2</v>
+      </c>
+      <c r="C11" s="4">
+        <v>9.8092643051771108E-2</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4918,7 +5785,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="B2" sqref="B2:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5151,6 +6018,244 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4988BB1E-D093-478C-9225-E5F9EEBFD2A3}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="6" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{559F736D-8FD6-46ED-9A45-F3CB0139281B}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -5387,242 +6492,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6250CC1C-01D0-42DD-AC51-C4DB5F2138AA}">
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="6" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.85</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.85</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.85</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0.85</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.85</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
working spreadsheet for edatopic adjustments for all species
</commit_message>
<xml_diff>
--- a/inputsGit/SI_percent_by_edagrid.xlsx
+++ b/inputsGit/SI_percent_by_edagrid.xlsx
@@ -1,44 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\SIBEC_Modelled\inputsGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DE4417-1044-4526-8C29-C486DAE1DDE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9A3910-2F41-4CAB-AC2F-ED00CF29A24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="56760" yWindow="1005" windowWidth="17685" windowHeight="18930" firstSheet="5" activeTab="13" xr2:uid="{C44777EE-7EF2-477D-9B72-BFFF0EC7632C}"/>
+    <workbookView xWindow="41625" yWindow="690" windowWidth="31350" windowHeight="19725" activeTab="4" xr2:uid="{C44777EE-7EF2-477D-9B72-BFFF0EC7632C}"/>
   </bookViews>
   <sheets>
     <sheet name="Ba" sheetId="10" r:id="rId1"/>
     <sheet name="Bg" sheetId="11" r:id="rId2"/>
     <sheet name="Bl" sheetId="9" r:id="rId3"/>
     <sheet name="Cw" sheetId="3" r:id="rId4"/>
-    <sheet name="Fd" sheetId="22" r:id="rId5"/>
-    <sheet name="Hm" sheetId="8" r:id="rId6"/>
-    <sheet name="Hw" sheetId="1" r:id="rId7"/>
-    <sheet name="La" sheetId="24" r:id="rId8"/>
-    <sheet name="Lw" sheetId="17" r:id="rId9"/>
-    <sheet name="Pa" sheetId="23" r:id="rId10"/>
-    <sheet name="Pl" sheetId="5" r:id="rId11"/>
-    <sheet name="Pw" sheetId="21" r:id="rId12"/>
-    <sheet name="Py" sheetId="7" r:id="rId13"/>
-    <sheet name="Sb" sheetId="25" r:id="rId14"/>
-    <sheet name="Ss" sheetId="2" r:id="rId15"/>
-    <sheet name="Sx" sheetId="6" r:id="rId16"/>
-    <sheet name="Yc" sheetId="15" r:id="rId17"/>
-    <sheet name="Ac" sheetId="14" r:id="rId18"/>
-    <sheet name="At" sheetId="18" r:id="rId19"/>
-    <sheet name="Dr" sheetId="12" r:id="rId20"/>
-    <sheet name="Ep" sheetId="13" r:id="rId21"/>
-    <sheet name="Mb" sheetId="16" r:id="rId22"/>
-    <sheet name="Ra" sheetId="19" r:id="rId23"/>
-    <sheet name="Bp" sheetId="20" r:id="rId24"/>
+    <sheet name="Fdi" sheetId="22" r:id="rId5"/>
+    <sheet name="Fdc" sheetId="26" r:id="rId6"/>
+    <sheet name="Hm" sheetId="8" r:id="rId7"/>
+    <sheet name="Hw" sheetId="1" r:id="rId8"/>
+    <sheet name="La" sheetId="24" r:id="rId9"/>
+    <sheet name="Lw" sheetId="17" r:id="rId10"/>
+    <sheet name="Pa" sheetId="23" r:id="rId11"/>
+    <sheet name="Pl" sheetId="5" r:id="rId12"/>
+    <sheet name="Pw" sheetId="21" r:id="rId13"/>
+    <sheet name="Py" sheetId="7" r:id="rId14"/>
+    <sheet name="Sb" sheetId="25" r:id="rId15"/>
+    <sheet name="Ss" sheetId="2" r:id="rId16"/>
+    <sheet name="Sx" sheetId="6" r:id="rId17"/>
+    <sheet name="Yc" sheetId="15" r:id="rId18"/>
+    <sheet name="Ac" sheetId="14" r:id="rId19"/>
+    <sheet name="At" sheetId="18" r:id="rId20"/>
+    <sheet name="Dr" sheetId="12" r:id="rId21"/>
+    <sheet name="Ep" sheetId="13" r:id="rId22"/>
+    <sheet name="Mb" sheetId="16" r:id="rId23"/>
+    <sheet name="Ra" sheetId="19" r:id="rId24"/>
+    <sheet name="Bp" sheetId="20" r:id="rId25"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +47,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -54,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="26">
   <si>
     <t>A</t>
   </si>
@@ -103,6 +109,36 @@
   <si>
     <t>aSMR</t>
   </si>
+  <si>
+    <t>Fdc</t>
+  </si>
+  <si>
+    <t>VR</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>VP</t>
+  </si>
+  <si>
+    <t>Using the Klinka and Carter equation</t>
+  </si>
+  <si>
+    <t>si_ratio</t>
+  </si>
+  <si>
+    <t>snr</t>
+  </si>
+  <si>
+    <t>asmr</t>
+  </si>
+  <si>
+    <t>spp</t>
+  </si>
 </sst>
 </file>
 
@@ -117,7 +153,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,6 +163,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -143,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -151,6 +193,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -166,6 +209,870 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Fdc!$Q$28:$Q$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Fdc!$R$28:$R$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>35.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0147-4B7A-BCB0-0BF91F0E6C0D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1286204767"/>
+        <c:axId val="1975278688"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1286204767"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1975278688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1975278688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1286204767"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -252,6 +1159,201 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4036A5CE-8AFC-470F-9C1B-F8D93C14B79F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9286875" y="1009650"/>
+          <a:ext cx="5924550" cy="2657475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>Klinka and Carter 2001. Relationships Between Coastal Douglas-fir Site Index and Synoptic</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>Categorical Measures of Site Quality</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1050" b="1"/>
+            <a:t> SI = 35.5 − 7.0(VD) − 1.4(MD) + 0.1(SD) + 3.1(F) + 0.0(M) − 9.4(VP) − 7.4(P) − 4.9(M) − 1.5(R) + 0.0(VR). </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>This equation had a adjusted R2 = 0.85, SEE = 2.0.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>This equation is probably published</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t> incorrectly and should be </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1050" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> SI = 35.5 − 7.0(VD) − 3.1 (MD) + 1.4(SD) + 0.1(F) + 0.0(M) − 9.4(VP) − 7.4(P) − 4.9(M) − 1.5(R) + 0.0(VR). </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-CA" sz="1050"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>Here we can assume that 35.5 meters is the climatic optimum for Fdc in the CWHxm.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>Does not cover ED,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t> XD, VM, or W.  Guess </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>XD = 18, ED = 35.5, VM = 12, W = 35.5</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-CA" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-CA" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>Probably the equation breaks down as the influence of drought or excessive moisture influences outweigh nutrient status. In the VD and MD ranges it is likely that the excessive drought hampers the ability to use the better nutrient status.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC393019-D677-403B-B5E1-8C471636E62F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -328,7 +1430,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -409,7 +1511,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1023,6 +2125,245 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{559F736D-8FD6-46ED-9A45-F3CB0139281B}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="6" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.35</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25F4FD76-F19D-40EF-915A-A0F6EB6E36A8}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -1260,7 +2601,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6250CC1C-01D0-42DD-AC51-C4DB5F2138AA}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -1498,7 +2839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4953CF86-436B-4117-96BF-9FCE03BF4B07}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -1733,7 +3074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0375AB61-F097-4CA1-BB9B-4DA4E8FB6CA1}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -1971,12 +3312,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A0336A-0F83-42F2-B3CC-E642C18C6FC6}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2209,7 +3550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07132632-98F5-41C9-B7B8-AE6846773071}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -2449,7 +3790,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE4AA88-8C45-4179-B9D3-DBCCEFC23EB4}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -2686,7 +4027,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95792EA-508C-4FAB-9880-E7E4A88B6EB9}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -2925,7 +4266,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3BD4163-0421-4FFD-95C4-3CE5C3514F0C}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -3136,244 +4477,6 @@
       </c>
       <c r="F10" s="4">
         <v>0.3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0663FF-CDCA-49DE-9890-01552EBC4BB4}">
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="6" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.65</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0.65</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.85</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="4">
-        <v>0.65</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0.85</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="4">
-        <v>0</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3641,6 +4744,244 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0663FF-CDCA-49DE-9890-01552EBC4BB4}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="6" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7531EF36-4035-4AFE-9241-025B586BB1A0}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -3878,7 +5219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D1A95C2-1624-41ED-ACAD-A32382F3B6BB}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -4116,7 +5457,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3172A72E-40EB-4724-8228-59CA56AA7FC6}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -4354,7 +5695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5277536-7F28-432C-B85E-FF4CDCE31DFD}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -4592,12 +5933,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8BCF85A-F29E-4B12-A803-7B01DEE1E39A}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F11"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5308,8 +6649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A36274-EA7F-44AE-83E3-428B3701CBE4}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5543,6 +6884,973 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18AF549-F393-4B95-A9EC-EB5AC5AEFB8D}">
+  <dimension ref="A1:R46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9">
+        <f>(35.5-7-9.4)/35.5</f>
+        <v>0.53802816901408457</v>
+      </c>
+      <c r="J9">
+        <f>(35.5-7-7.4)/35.5</f>
+        <v>0.59436619718309858</v>
+      </c>
+      <c r="K9" s="5">
+        <f>(35.5-7-4.9)/35.5</f>
+        <v>0.6647887323943662</v>
+      </c>
+      <c r="L9" s="5">
+        <f>(35.5-7-1.5)/35.5</f>
+        <v>0.76056338028169013</v>
+      </c>
+      <c r="M9" s="5">
+        <f>(35.5-7-0)/35.5</f>
+        <v>0.80281690140845074</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <f>(35.5-3.1-9.4)/35.5</f>
+        <v>0.647887323943662</v>
+      </c>
+      <c r="J10">
+        <f>(35.5-3.1-7.4)/35.5</f>
+        <v>0.70422535211267601</v>
+      </c>
+      <c r="K10">
+        <f>(35.5-3.1-4.9)/35.5</f>
+        <v>0.77464788732394363</v>
+      </c>
+      <c r="L10">
+        <f>(35.5-3.1-1.5)/35.5</f>
+        <v>0.87042253521126756</v>
+      </c>
+      <c r="M10">
+        <f>(35.5-3.1-0)/35.5</f>
+        <v>0.91267605633802817</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11">
+        <f>(35.5-1.4-9.4)/35.5</f>
+        <v>0.69577464788732402</v>
+      </c>
+      <c r="J11">
+        <f>(35.5-1.4-7.4)/35.5</f>
+        <v>0.75211267605633814</v>
+      </c>
+      <c r="K11">
+        <f>(35.5-1.4-4.9)/35.5</f>
+        <v>0.82253521126760576</v>
+      </c>
+      <c r="L11">
+        <f>(35.5-1.4- 1.5)/35.5</f>
+        <v>0.91830985915492958</v>
+      </c>
+      <c r="M11">
+        <f>(35.5-1.4-0)/35.5</f>
+        <v>0.96056338028169019</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <f>(35.5-0.1-9.4)/35.5</f>
+        <v>0.73239436619718312</v>
+      </c>
+      <c r="J12">
+        <f>(35.5-0.1-7.4)/35.5</f>
+        <v>0.78873239436619713</v>
+      </c>
+      <c r="K12">
+        <f>(35.5-0.1-4.9)/35.5</f>
+        <v>0.85915492957746475</v>
+      </c>
+      <c r="L12">
+        <f>(35.5-0.1-1.5)/35.5</f>
+        <v>0.95492957746478868</v>
+      </c>
+      <c r="M12">
+        <f>(35.5-0.1-0)/35.5</f>
+        <v>0.9971830985915493</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0.59436619718309858</v>
+      </c>
+      <c r="G13">
+        <v>6</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13">
+        <f>(35.5-0-9.4)/35.5</f>
+        <v>0.73521126760563382</v>
+      </c>
+      <c r="J13">
+        <f>(35.5-0-7.4)/35.5</f>
+        <v>0.79154929577464794</v>
+      </c>
+      <c r="K13">
+        <f>(35.5-0-4.9)/35.5</f>
+        <v>0.86197183098591557</v>
+      </c>
+      <c r="L13">
+        <f>(35.5-0-1.5)/35.5</f>
+        <v>0.95774647887323938</v>
+      </c>
+      <c r="M13">
+        <f>(35.5-0-0)/35.5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>0.6647887323943662</v>
+      </c>
+      <c r="G14">
+        <v>7</v>
+      </c>
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>0.76056338028169013</v>
+      </c>
+      <c r="G15">
+        <v>8</v>
+      </c>
+      <c r="H15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>0.80281690140845074</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0.647887323943662</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0.70422535211267601</v>
+      </c>
+      <c r="I18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" t="s">
+        <v>18</v>
+      </c>
+      <c r="M18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>0.77464788732394363</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>0.87042253521126756</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>0.91267605633802817</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21">
+        <v>0.53802816901408457</v>
+      </c>
+      <c r="J21">
+        <v>0.59436619718309858</v>
+      </c>
+      <c r="K21">
+        <v>0.6647887323943662</v>
+      </c>
+      <c r="L21">
+        <v>0.76056338028169013</v>
+      </c>
+      <c r="M21">
+        <v>0.80281690140845074</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0.69577464788732402</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22">
+        <v>0.647887323943662</v>
+      </c>
+      <c r="J22">
+        <v>0.70422535211267601</v>
+      </c>
+      <c r="K22">
+        <v>0.77464788732394363</v>
+      </c>
+      <c r="L22">
+        <v>0.87042253521126756</v>
+      </c>
+      <c r="M22">
+        <v>0.91267605633802817</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0.75211267605633814</v>
+      </c>
+      <c r="G23">
+        <v>4</v>
+      </c>
+      <c r="H23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23">
+        <v>0.69577464788732402</v>
+      </c>
+      <c r="J23">
+        <v>0.75211267605633814</v>
+      </c>
+      <c r="K23">
+        <v>0.82253521126760576</v>
+      </c>
+      <c r="L23">
+        <v>0.91830985915492958</v>
+      </c>
+      <c r="M23">
+        <v>0.96056338028169019</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>0.82253521126760576</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="H24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24">
+        <v>0.73239436619718312</v>
+      </c>
+      <c r="J24">
+        <v>0.78873239436619713</v>
+      </c>
+      <c r="K24">
+        <v>0.85915492957746475</v>
+      </c>
+      <c r="L24">
+        <v>0.95492957746478868</v>
+      </c>
+      <c r="M24">
+        <v>0.9971830985915493</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>0.91830985915492958</v>
+      </c>
+      <c r="G25">
+        <v>6</v>
+      </c>
+      <c r="H25" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25">
+        <v>0.73521126760563382</v>
+      </c>
+      <c r="J25">
+        <v>0.79154929577464794</v>
+      </c>
+      <c r="K25">
+        <v>0.86197183098591557</v>
+      </c>
+      <c r="L25">
+        <v>0.95774647887323938</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>0.96056338028169019</v>
+      </c>
+      <c r="G26">
+        <v>7</v>
+      </c>
+      <c r="H26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0.73239436619718312</v>
+      </c>
+      <c r="G27">
+        <v>8</v>
+      </c>
+      <c r="H27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>0.78873239436619713</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>35.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>0.85915492957746475</v>
+      </c>
+      <c r="Q29">
+        <v>1</v>
+      </c>
+      <c r="R29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>0.95492957746478868</v>
+      </c>
+      <c r="Q30">
+        <v>2</v>
+      </c>
+      <c r="R30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31">
+        <v>0.9971830985915493</v>
+      </c>
+      <c r="Q31">
+        <v>3</v>
+      </c>
+      <c r="R31">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0.73521126760563382</v>
+      </c>
+      <c r="Q32">
+        <v>4</v>
+      </c>
+      <c r="R32">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0.79154929577464794</v>
+      </c>
+      <c r="Q33">
+        <v>5</v>
+      </c>
+      <c r="R33">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>0.86197183098591557</v>
+      </c>
+      <c r="Q34">
+        <v>6</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>0.95774647887323938</v>
+      </c>
+      <c r="Q35">
+        <v>7</v>
+      </c>
+      <c r="R35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="Q36">
+        <v>8</v>
+      </c>
+      <c r="R36">
+        <v>35.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42">
+        <v>8</v>
+      </c>
+      <c r="C42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46">
+        <v>8</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B7A8035-D1C6-449D-9E31-0C0026591847}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -5780,7 +8088,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14A8E0C9-6120-4EDE-A504-D2BABBC45675}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -6017,7 +8325,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4988BB1E-D093-478C-9225-E5F9EEBFD2A3}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -6253,243 +8561,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{559F736D-8FD6-46ED-9A45-F3CB0139281B}">
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="6" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0.35</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.65</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.65</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.85</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="4">
-        <v>0.85</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.65</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.65</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>